<commit_message>
Lab 5 actualizado  (#2)
* Primeros cambios

* fix tests

* Carpeta Docs

* README actualizado
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 5.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 5.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linds\Desktop\Liv-stuff\MAESTRIA\PRIMER SEMESTRE\ASISTENCIA\Lab 5 def\ISIS1225-Laboratorio-5\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lina/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB75D800-80A7-4AAA-AE7C-4DF4FF1189B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6DE5ECC-B753-4C4F-8EF0-1FF87AB8F3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="01-Data Lab 5" sheetId="1" r:id="rId1"/>
-    <sheet name="02-ARRAY_LIST" sheetId="6" r:id="rId2"/>
-    <sheet name="03-LINKED_LIST" sheetId="13" r:id="rId3"/>
-    <sheet name="04-Selection Sort" sheetId="8" r:id="rId4"/>
-    <sheet name="05-Merge Sort" sheetId="14" r:id="rId5"/>
+    <sheet name="01-Data Lab 4" sheetId="1" r:id="rId1"/>
+    <sheet name="02-Insertion Sort" sheetId="8" r:id="rId2"/>
+    <sheet name="03-Selection Sort" sheetId="14" r:id="rId3"/>
+    <sheet name="04-Shell Sort" sheetId="26" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,35 +39,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Porcentaje de la muestra [pct]</t>
   </si>
   <si>
-    <r>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Dax-Regular"/>
-      </rPr>
-      <t>amaño de la muestra (ARRAY_LIST)</t>
-    </r>
+    <t>Tamaño de la muestra (ARRAY_LIST)</t>
   </si>
   <si>
     <t>Tamaño de la muestra (LINKED_LIST)</t>
   </si>
   <si>
-    <t>Column1</t>
+    <t>Tamaño de la muestra (especificar array o linked)</t>
   </si>
   <si>
-    <t>Selection Sort [ms]</t>
+    <t>TIEMPOS DE EJECUCIÓN INSERTION SORT[ms]</t>
   </si>
   <si>
-    <t>Merge Sort [ms]</t>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Array List</t>
+  </si>
+  <si>
+    <t>TIEMPOS DE EJECUCIÓN SELECTION SORT[ms]</t>
+  </si>
+  <si>
+    <t>TIEMPOS DE EJECUCIÓN SHELL SORT[ms]</t>
   </si>
 </sst>
 </file>
@@ -109,30 +107,56 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Dax-Regular"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Dax-Regular"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF69E76"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC1F8F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -140,50 +164,246 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -193,22 +413,25 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="0"/>
+        <color rgb="FF000000"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -218,66 +441,10 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -296,17 +463,21 @@
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -316,17 +487,10 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="0"/>
+        <color rgb="FF000000"/>
         <name val="Dax-Regular"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -427,8 +591,130 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC1F8F3"/>
+      <color rgb="FF7FF9EA"/>
+      <color rgb="FF73FDD6"/>
+      <color rgb="FFF69E76"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -443,1691 +729,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-419" sz="1800" b="1">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Comparación de tiempos de ejecucion con ARRAY_LIST</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1800" b="1">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.2031634608723763"/>
-          <c:y val="1.2121212121212121E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.1237011337659039"/>
-          <c:y val="0.1332829078183409"/>
-          <c:w val="0.84440367608007938"/>
-          <c:h val="0.74534303666587132"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'01-Data Lab 5'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Selection Sort [ms]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.11909541182718729"/>
-                  <c:y val="-2.3553328561202503E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$C$2:$C$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EA19-4908-9336-CD0E2C6ECFDA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'01-Data Lab 5'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Merge Sort [ms]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-5.0620549569061354E-2"/>
-                  <c:y val="-3.5983545576759562E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$D$2:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-50BD-409F-AD4F-AE6565325CF2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'01-Data Lab 5'!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Column1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$E$2:$E$10</c:f>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-0662-4A10-BB27-BF2CF30161F7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="696671312"/>
-        <c:axId val="1833162896"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="696671312"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>Tamaño</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" b="1" baseline="0"/>
-                  <a:t> de la muestra [Num. Elementos]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" b="1"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1833162896"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1833162896"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>Tiempo</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" b="1" baseline="0"/>
-                  <a:t> de ejecución [ms]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" b="1"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="696671312"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.4324243193940923E-2"/>
-          <c:y val="0.91893867811978047"/>
-          <c:w val="0.95774447548895103"/>
-          <c:h val="6.8940109759007398E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-419" sz="1800" b="1">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Comparación de tiempos de ejecucion con LINKED_LIST</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1800" b="1">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.2031634608723763"/>
-          <c:y val="1.2121212121212121E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.1237011337659039"/>
-          <c:y val="0.1332829078183409"/>
-          <c:w val="0.84440367608007938"/>
-          <c:h val="0.74534303666587132"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'01-Data Lab 5'!$C$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Selection Sort [ms]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.11909541182718729"/>
-                  <c:y val="-2.3553328561202503E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$13:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$C$13:$C$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7ACA-4F6D-A3D9-CBDDAE5EDD6E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'01-Data Lab 5'!$D$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Merge Sort [ms]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-8.8759881488552017E-2"/>
-                  <c:y val="-2.9996501429511446E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$13:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$D$13:$D$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7ACA-4F6D-A3D9-CBDDAE5EDD6E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'01-Data Lab 5'!$E$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Column1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$13:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'01-Data Lab 5'!$E$13:$E$20</c:f>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-7ACA-4F6D-A3D9-CBDDAE5EDD6E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="696671312"/>
-        <c:axId val="1833162896"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="696671312"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>Tamaño</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" b="1" baseline="0"/>
-                  <a:t> de la muestra [Num. Elementos]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" b="1"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1833162896"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1833162896"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>Tiempo</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" b="1" baseline="0"/>
-                  <a:t> de ejecución [ms]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" b="1"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="696671312"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.4324243193940923E-2"/>
-          <c:y val="0.91893867811978047"/>
-          <c:w val="0.95774447548895103"/>
-          <c:h val="6.8940109759007398E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2163,7 +765,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> Selection Sort</a:t>
+              <a:t> Insertion Sort</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
@@ -2209,11 +811,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01-Data Lab 5'!$C$1</c:f>
+              <c:f>'01-Data Lab 4'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Selection Sort [ms]</c:v>
+                  <c:v>Array List</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2294,10 +896,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$2:$A$10</c:f>
+              <c:f>'01-Data Lab 4'!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
@@ -2327,10 +929,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'01-Data Lab 5'!$C$2:$C$10</c:f>
+              <c:f>'01-Data Lab 4'!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2346,11 +948,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01-Data Lab 5'!$C$12</c:f>
+              <c:f>'01-Data Lab 4'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Selection Sort [ms]</c:v>
+                  <c:v>Linked List</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2431,7 +1033,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$13:$A$20</c:f>
+              <c:f>'01-Data Lab 4'!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2464,7 +1066,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'01-Data Lab 5'!$C$13:$C$20</c:f>
+              <c:f>'01-Data Lab 4'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2806,10 +1408,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2845,9 +1447,12 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t> Merge Sort</a:t>
+              <a:t> Selection</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t> Sort</a:t>
+            </a:r>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2891,11 +1496,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01-Data Lab 5'!$D$1</c:f>
+              <c:f>'01-Data Lab 4'!$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Merge Sort [ms]</c:v>
+                  <c:v>Array List</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2976,10 +1581,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$2:$A$10</c:f>
+              <c:f>'01-Data Lab 4'!$A$14:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
@@ -3009,10 +1614,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'01-Data Lab 5'!$D$2:$D$10</c:f>
+              <c:f>'01-Data Lab 4'!$C$14:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3028,11 +1633,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'01-Data Lab 5'!$D$12</c:f>
+              <c:f>'01-Data Lab 4'!$D$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Merge Sort [ms]</c:v>
+                  <c:v>Linked List</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3113,7 +1718,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'01-Data Lab 5'!$A$13:$A$20</c:f>
+              <c:f>'01-Data Lab 4'!$A$14:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3146,7 +1751,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'01-Data Lab 5'!$D$13:$D$20</c:f>
+              <c:f>'01-Data Lab 4'!$D$14:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3157,6 +1762,688 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-80E6-4C96-B542-B32CC3AB919F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1328118000"/>
+        <c:axId val="1328121328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1328118000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tamaño</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> de la muestra [Num. elementos]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328121328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1328121328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Tiempo de Ejecución [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1328118000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Comparación de tiempos de ejecucion Sell</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> Sort</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'01-Data Lab 4'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Array List</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1363811854896437"/>
+                  <c:y val="-3.2945200031814204E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$H$3:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-593D-443F-9CD6-04EF414BEDDD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'01-Data Lab 4'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linked List</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.593553005287829E-2"/>
+                  <c:y val="0.12376727909011373"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'01-Data Lab 4'!$I$3:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-593D-443F-9CD6-04EF414BEDDD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3608,46 +2895,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5196,547 +4443,11 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EAD1D623-F0B6-4C1A-913F-35E2F001B69E}">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FFC1F8F3"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5745,9 +4456,24 @@
 </chartsheet>
 </file>
 
-<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EF2FF808-7ED0-47FB-B864-504F6F16AA8A}">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B1BECD7C-0E68-4F70-B3B6-C22C36A0C26A}">
+  <sheetPr>
+    <tabColor rgb="FFF69E76"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5760,73 +4486,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672454" cy="6279444"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F86A8C9-B823-4237-B971-35F9FC141626}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672454" cy="6279444"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D209CB7-6B9C-47D1-9CA7-0D240F42F3EA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672513" cy="6281738"/>
+    <xdr:ext cx="8674100" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5855,11 +4515,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8672513" cy="6281738"/>
+    <xdr:ext cx="8674100" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5888,40 +4548,81 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8674100" cy="6286500"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9B0B28A-DE5E-E347-1DCC-EBC3E818A846}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:E9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:E9" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Porcentaje de la muestra [pct]" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tamaño de la muestra (ARRAY_LIST)" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:D10" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A2:D10" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Porcentaje de la muestra [pct]" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tamaño de la muestra (ARRAY_LIST)" dataDxfId="8">
       <calculatedColumnFormula>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Selection Sort [ms]"/>
-    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Merge Sort [ms]"/>
-    <tableColumn id="5" xr3:uid="{61DF25D7-A2A3-4D39-B0C6-29804C1B33DB}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Array List" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{56471E76-DCC6-4EED-8237-BCC256B57E91}" name="Linked List" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A12:E20" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A12:E20" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Porcentaje de la muestra [pct]" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A13:D21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A13:D21" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Porcentaje de la muestra [pct]" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="4">
       <calculatedColumnFormula>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Selection Sort [ms]"/>
-    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Merge Sort [ms]"/>
-    <tableColumn id="5" xr3:uid="{EE99E4CD-A6F0-492B-B754-38221659D42F}" name="Column1" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Array List" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A5E99D51-DD73-48A7-AE0D-601A8EE89AFA}" name="Linked List" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -6217,248 +4918,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.46484375" style="8" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" style="3" customWidth="1"/>
+    <col min="6" max="12" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="27.75">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="F1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="33" thickBot="1">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="H2" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="13.9">
-      <c r="A2" s="10">
+    <row r="3" spans="1:9" s="2" customFormat="1">
+      <c r="A3" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B3" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="12"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G3" s="15">
+        <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>50</v>
+      </c>
+      <c r="H3" s="33"/>
+      <c r="I3" s="34"/>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="13.9">
-      <c r="A3" s="10">
+    <row r="4" spans="1:9" s="2" customFormat="1">
+      <c r="A4" s="8">
         <v>0.05</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B4" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>500</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="12"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="5">
+        <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>500</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="17"/>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2">
+    <row r="5" spans="1:9">
+      <c r="A5" s="8">
         <v>0.1</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="7"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="15">
+        <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>1000</v>
+      </c>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="10">
+    <row r="6" spans="1:9">
+      <c r="A6" s="8">
         <v>0.2</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B6" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>2000</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="12"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="5">
+        <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>2000</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="17"/>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2">
+    <row r="7" spans="1:9">
+      <c r="A7" s="8">
         <v>0.3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="7"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="15">
+        <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>3000</v>
+      </c>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2">
+    <row r="8" spans="1:9">
+      <c r="A8" s="8">
         <v>0.5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>5000</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="5">
+        <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>5000</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="17"/>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2">
+    <row r="9" spans="1:9">
+      <c r="A9" s="8">
         <v>0.8</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="5">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="7"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="15">
+        <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>8000</v>
+      </c>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2">
+    <row r="10" spans="1:9" ht="16" thickBot="1">
+      <c r="A10" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="11">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="7"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="11">
+        <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
+        <v>10000</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="18"/>
     </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="27.75">
-      <c r="A12" s="4" t="s">
+    <row r="11" spans="1:9" ht="16" thickBot="1">
+      <c r="E11"/>
+    </row>
+    <row r="12" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A12" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="32">
+      <c r="A13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" ht="13.9">
-      <c r="A13" s="10">
+    <row r="14" spans="1:9" s="2" customFormat="1">
+      <c r="A14" s="8">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B14" s="5">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="12"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="9"/>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="13.9">
-      <c r="A14" s="10">
+    <row r="15" spans="1:9" s="2" customFormat="1">
+      <c r="A15" s="8">
         <v>0.05</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B15" s="5">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>500</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="12"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="9"/>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2">
+    <row r="16" spans="1:9">
+      <c r="A16" s="8">
         <v>0.1</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="5">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="9"/>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="10">
+    <row r="17" spans="1:9">
+      <c r="A17" s="8">
         <v>0.2</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B17" s="5">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>2000</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="12"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="9"/>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2">
+    <row r="18" spans="1:9">
+      <c r="A18" s="8">
         <v>0.3</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B18" s="5">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="7"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="9"/>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2">
+    <row r="19" spans="1:9">
+      <c r="A19" s="8">
         <v>0.5</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B19" s="5">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>5000</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="7"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="9"/>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2">
+    <row r="20" spans="1:9">
+      <c r="A20" s="8">
         <v>0.8</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="5">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="7"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="9"/>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="2">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
+      <c r="A21" s="10">
         <v>1</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B21" s="11">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="7"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F12:I12"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
@@ -6468,8 +5319,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="af74a0f8eb440a60883e9dd833f0742f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5ceeff32ffca1089660572a8ebd1782" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4e7eefc5f66e7d51449543297ddde059">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df8efc3b1b447b14ec56bc155bd746d7" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
     <xsd:import namespace="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
     <xsd:element name="properties">
@@ -6558,7 +5409,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a38e7027-190f-4f90-8839-9f8250567d86" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a38e7027-190f-4f90-8839-9f8250567d86" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -6579,7 +5430,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="85e30bcc-d76c-4413-8e4d-2dce22fb0743" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -6598,7 +5449,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -6626,8 +5477,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -6717,15 +5568,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
@@ -6838,8 +5680,17 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24D72429-8592-4E2D-9A60-DFD77A3B0B84}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BEEE7F2-DD9A-42EF-8F73-A92FC7ED8D52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -6858,26 +5709,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>